<commit_message>
added field type in file data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/Datasheet.xlsx
+++ b/src/test/resources/Datasheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giris\eclipse-workspace\forms\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4186DFF-7D4B-47FA-961E-18CC364140FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5846B9B-3909-496F-A275-2C4E36546B2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6620" xr2:uid="{E7E473B2-BFC6-486D-91AE-5DF6880DC63C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>edit-submitted-event-form-fname</t>
   </si>
@@ -39,10 +39,25 @@
     <t>lllll</t>
   </si>
   <si>
-    <t>textfield</t>
-  </si>
-  <si>
     <t>lov</t>
+  </si>
+  <si>
+    <t>edit-submitted-event-form-title</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -393,39 +408,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31FB389-1EE7-4B55-98D3-1BA1C7606638}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE3161-A045-445D-B5D9-5C44AC855FB3}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="29.953125" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
+    <col min="1" max="1" width="35.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
+      <c r="D1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
         <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>